<commit_message>
add STU 2.0, fix spreadsheet issues
</commit_message>
<xml_diff>
--- a/lib/smart_app_launch/requirements/hl7.fhir.uv.smart-app-launch_2.2.0_Requirements.xlsx
+++ b/lib/smart_app_launch/requirements/hl7.fhir.uv.smart-app-launch_2.2.0_Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/smart-app-launch-test-kit/lib/smart_app_launch/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7966395-9388-244E-ABE1-FF478206F1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD794982-FDDE-2F47-8747-F01370F818DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="606">
   <si>
     <r>
       <rPr>
@@ -3277,6 +3277,12 @@
       </rPr>
       <t>E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.</t>
     </r>
+  </si>
+  <si>
+    <t>[When responding to a `/.well-known/smart-configuration` request the] ...Metadata ...`registration_endpoint`[is] RECOMMENDED … [and Shall contain the] URL to the OAuth2 dynamic registration endpoint for this FHIR server.</t>
+  </si>
+  <si>
+    <t>[When responding to a `/.well-known/smart-configuration` request the] ...Metadata ...`associated_endpoints`[is] RECOMMENDED … [and Shall contain an a]rray of objects for endpoints that share the same authorization mechanism as this FHIR endpoint, each with a “url” and “capabilities” array.</t>
   </si>
 </sst>
 </file>
@@ -4197,10 +4203,10 @@
   <dimension ref="A1:AC493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G359" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomRight" activeCell="B441" sqref="B441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14556,24 +14562,54 @@
         <v>must-support-definition-ms-and-data-absent-reasons</v>
       </c>
     </row>
-    <row r="439" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A439" s="2">
+        <v>438</v>
+      </c>
+      <c r="B439" s="35" t="s">
+        <v>506</v>
+      </c>
+      <c r="C439" s="37" t="s">
+        <v>604</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E439" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="M439" s="34" t="str" cm="1">
         <f t="array" ref="M439">PAGE_NAME(B439)</f>
-        <v/>
+        <v>conformance</v>
       </c>
       <c r="N439" s="34" t="str" cm="1">
         <f t="array" ref="N439">SECTION_NAME(B439)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="440" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>metadata</v>
+      </c>
+    </row>
+    <row r="440" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A440" s="2">
+        <v>439</v>
+      </c>
+      <c r="B440" s="35" t="s">
+        <v>506</v>
+      </c>
+      <c r="C440" s="37" t="s">
+        <v>605</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E440" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="M440" s="34" t="str" cm="1">
         <f t="array" ref="M440">PAGE_NAME(B440)</f>
-        <v/>
+        <v>conformance</v>
       </c>
       <c r="N440" s="34" t="str" cm="1">
         <f t="array" ref="N440">SECTION_NAME(B440)</f>
-        <v/>
+        <v>metadata</v>
       </c>
     </row>
     <row r="441" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -15443,6 +15479,8 @@
     <hyperlink ref="B370" r:id="rId331" location="capabilities" xr:uid="{72CA9D63-D43C-4229-9F85-1C384B13A10D}"/>
     <hyperlink ref="B371" r:id="rId332" location="capabilities" xr:uid="{2361F186-8347-42A8-81D0-F310B08B7355}"/>
     <hyperlink ref="B372" r:id="rId333" location="capabilities" xr:uid="{E41379CF-D4D2-4DC5-A897-7DE0ABFCFFFD}"/>
+    <hyperlink ref="B439" r:id="rId334" location="metadata" xr:uid="{959D4FCD-6A00-2E41-9FDB-C463D8EFD09A}"/>
+    <hyperlink ref="B440" r:id="rId335" location="metadata" xr:uid="{E1AE3417-D87F-284B-949F-2B1ED9F2602A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -15452,19 +15490,19 @@
           <x14:formula1>
             <xm:f>'Column Data'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G1:G438 G441:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4866B9BF-5615-6646-965F-909D4D65F2A5}">
           <x14:formula1>
             <xm:f>'Column Data'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D438 D441:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4FB27A2-804E-CB49-B85C-BBEE0C688B4F}">
           <x14:formula1>
             <xm:f>'Column Data'!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576 I2:I1048576</xm:sqref>
+          <xm:sqref>I441:I1048576 I2:I438 K2:K438 K441:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15708,12 +15746,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15971,22 +16013,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16012,12 +16053,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>